<commit_message>
update summarised mapping stats.
</commit_message>
<xml_diff>
--- a/files/SI_Data_1__CS_3endRNASeq.xlsx
+++ b/files/SI_Data_1__CS_3endRNASeq.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsun/Google Drive/research/wheat_tagseq/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsun/Google Drive/projects/HuoberBrezel/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C758662F-AB67-5C4F-A1EC-AA2D21208C93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6724C6E8-9B3D-1849-8A25-A33272BFC72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="6900" windowWidth="26960" windowHeight="11000" activeTab="1" xr2:uid="{0A1B866E-BAB2-5B48-9BA1-056163FF4A88}"/>
+    <workbookView xWindow="47500" yWindow="640" windowWidth="31980" windowHeight="13240" activeTab="1" xr2:uid="{0A1B866E-BAB2-5B48-9BA1-056163FF4A88}"/>
   </bookViews>
   <sheets>
     <sheet name="Trimmomatic" sheetId="2" r:id="rId1"/>
-    <sheet name="HISAT" sheetId="1" r:id="rId2"/>
-    <sheet name="EAGLE-RC" sheetId="3" r:id="rId3"/>
+    <sheet name="HISAT2" sheetId="1" r:id="rId2"/>
+    <sheet name="STAR" sheetId="4" r:id="rId3"/>
+    <sheet name="EAGLE-RC" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>library name</t>
   </si>
@@ -170,6 +171,21 @@
   </si>
   <si>
     <t>time [min/1M reads]</t>
+  </si>
+  <si>
+    <t>single-edn 126 bp</t>
+  </si>
+  <si>
+    <t>%F</t>
+  </si>
+  <si>
+    <t>% homeolog reads</t>
+  </si>
+  <si>
+    <t>* percentage of input reads that classified as A, B, D-origin</t>
+  </si>
+  <si>
+    <t>* F: percentage of reads that uniquely mapped on one of A, B, D subgenomes.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +198,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -205,6 +221,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +236,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -280,6 +302,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -308,8 +341,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -329,9 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -342,6 +371,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -661,12 +694,13 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="2" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -703,11 +737,11 @@
         <v>2604973</v>
       </c>
       <c r="E2" s="16">
-        <v>2078810</v>
+        <v>2052039</v>
       </c>
       <c r="F2" s="17">
         <f>E2/D2</f>
-        <v>0.79801594872576409</v>
+        <v>0.78773906677727557</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -724,11 +758,11 @@
         <v>1596414</v>
       </c>
       <c r="E3" s="7">
-        <v>1241292</v>
+        <v>1225463</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F7" si="0">E3/D3</f>
-        <v>0.77755018435067591</v>
+        <v>0.76763483657747933</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -745,11 +779,11 @@
         <v>3694206</v>
       </c>
       <c r="E4" s="7">
-        <v>2874064</v>
+        <v>2840365</v>
       </c>
       <c r="F4" s="8">
         <f t="shared" si="0"/>
-        <v>0.77799234801740891</v>
+        <v>0.76887022542868477</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -766,11 +800,11 @@
         <v>1764702</v>
       </c>
       <c r="E5" s="7">
-        <v>1393116</v>
+        <v>1374577</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" si="0"/>
-        <v>0.78943413675510088</v>
+        <v>0.77892868030976337</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -787,11 +821,11 @@
         <v>4347049</v>
       </c>
       <c r="E6" s="7">
-        <v>3385387</v>
+        <v>3340992</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" si="0"/>
-        <v>0.77877820102786977</v>
+        <v>0.76856552571641135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -807,12 +841,12 @@
       <c r="D7" s="12">
         <v>4122508</v>
       </c>
-      <c r="E7" s="25">
-        <v>3217619</v>
+      <c r="E7" s="23">
+        <v>3176144</v>
       </c>
       <c r="F7" s="13">
         <f t="shared" si="0"/>
-        <v>0.78050036531160161</v>
+        <v>0.7704397420211192</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -825,11 +859,11 @@
       </c>
       <c r="E8" s="20">
         <f t="shared" ref="E8:F8" si="1">AVERAGE(E2:E7)</f>
-        <v>2365048</v>
+        <v>2334930</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>0.78371186403140358</v>
+        <v>0.7736963461384555</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -844,11 +878,11 @@
       </c>
       <c r="E9" s="19">
         <f t="shared" ref="E9:F9" si="2">STDEV(E2:E7)</f>
-        <v>929137.00023430341</v>
+        <v>917440.84359090973</v>
       </c>
       <c r="F9" s="13">
         <f t="shared" si="2"/>
-        <v>8.2787095449685932E-3</v>
+        <v>8.0192200576312857E-3</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +892,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F027D-97EE-8C45-84CC-12021653609C}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -872,64 +906,70 @@
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="7" width="17.33203125" customWidth="1"/>
-    <col min="9" max="11" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" customWidth="1"/>
+    <col min="10" max="12" width="20.33203125" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="Q1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="R1" s="24" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S1" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
@@ -940,56 +980,64 @@
         <v>20</v>
       </c>
       <c r="D2" s="4">
-        <v>2078810</v>
+        <v>2052039</v>
       </c>
       <c r="E2" s="4">
-        <v>421594</v>
+        <v>418957</v>
       </c>
       <c r="F2" s="4">
-        <v>1221774</v>
+        <v>1204186</v>
       </c>
       <c r="G2" s="4">
-        <f t="shared" ref="G2:G7" si="0">D2-F2-E2</f>
-        <v>435442</v>
+        <f>D2-F2-E2</f>
+        <v>428896</v>
       </c>
       <c r="H2" s="3">
-        <f>F2/(F2+G2)</f>
-        <v>0.73724487332972888</v>
-      </c>
-      <c r="I2" s="4">
-        <v>401929</v>
+        <f>F2/D2</f>
+        <v>0.58682412956089036</v>
+      </c>
+      <c r="I2" s="3">
+        <f>F2/D2</f>
+        <v>0.58682412956089036</v>
       </c>
       <c r="J2" s="4">
-        <v>401174</v>
+        <v>396243</v>
       </c>
       <c r="K2" s="4">
-        <v>401553</v>
-      </c>
-      <c r="L2" s="3">
-        <f t="shared" ref="L2:N7" si="1">I2/($I2+$J2+$K2)</f>
-        <v>0.33364628574464411</v>
+        <v>395482</v>
+      </c>
+      <c r="L2" s="4">
+        <v>395536</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33301955080952572</v>
+        <f t="shared" ref="M2:O7" si="0">J2/($J2+$K2+$L2)</f>
+        <v>0.33374548646001173</v>
       </c>
       <c r="N2" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33333416344583017</v>
-      </c>
-      <c r="O2" s="21">
-        <v>34.76</v>
-      </c>
-      <c r="P2" s="29">
-        <f>O2/D2*1000000</f>
-        <v>16.721104862878281</v>
-      </c>
-      <c r="Q2" s="29">
-        <f>P2/60</f>
-        <v>0.27868508104797135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.33310451535087904</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33314999818910923</v>
+      </c>
+      <c r="P2">
+        <v>34.564</v>
+      </c>
+      <c r="Q2" s="27">
+        <f>P2/D2*1000000</f>
+        <v>16.843734451440735</v>
+      </c>
+      <c r="R2" s="27">
+        <f>Q2/60</f>
+        <v>0.28072890752401225</v>
+      </c>
+      <c r="S2" s="3">
+        <f>(J2+K2+L2)/D2</f>
+        <v>0.57857623563684701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1000,56 +1048,64 @@
         <v>20</v>
       </c>
       <c r="D3" s="4">
-        <v>1241292</v>
+        <v>1225463</v>
       </c>
       <c r="E3" s="4">
-        <v>222471</v>
+        <v>220835</v>
       </c>
       <c r="F3" s="4">
-        <v>748697</v>
+        <v>737997</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" si="0"/>
-        <v>270124</v>
+        <f>D3-F3-E3</f>
+        <v>266631</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H7" si="2">F3/(F3+G3)</f>
-        <v>0.73486608540656306</v>
-      </c>
-      <c r="I3" s="4">
-        <v>245739</v>
+        <f t="shared" ref="H3:H7" si="1">F3/D3</f>
+        <v>0.60221891644219372</v>
+      </c>
+      <c r="I3" s="3">
+        <f>F3/D3</f>
+        <v>0.60221891644219372</v>
       </c>
       <c r="J3" s="4">
-        <v>246833</v>
+        <v>242365</v>
       </c>
       <c r="K3" s="4">
-        <v>247368</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33210665729653754</v>
+        <v>243385</v>
+      </c>
+      <c r="L3" s="4">
+        <v>243636</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33358515555315293</v>
+        <f t="shared" si="0"/>
+        <v>0.332286333985023</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33430818715030947</v>
-      </c>
-      <c r="O3" s="21">
-        <v>27.609000000000002</v>
-      </c>
-      <c r="P3" s="29">
-        <f t="shared" ref="P3:P7" si="3">O3/D3*1000000</f>
-        <v>22.242147697721407</v>
-      </c>
-      <c r="Q3" s="29">
-        <f>P3/60</f>
-        <v>0.37070246162869014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.33368477047818301</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33402889553679393</v>
+      </c>
+      <c r="P3">
+        <v>28.119</v>
+      </c>
+      <c r="Q3" s="27">
+        <f t="shared" ref="Q3:Q7" si="2">P3/D3*1000000</f>
+        <v>22.945613209048336</v>
+      </c>
+      <c r="R3" s="27">
+        <f>Q3/60</f>
+        <v>0.38242688681747228</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S5" si="3">(J3+K3+L3)/D3</f>
+        <v>0.59519218450495859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1060,56 +1116,64 @@
         <v>20</v>
       </c>
       <c r="D4" s="4">
-        <v>2874064</v>
+        <v>2840365</v>
       </c>
       <c r="E4" s="4">
-        <v>558418</v>
+        <v>554927</v>
       </c>
       <c r="F4" s="4">
-        <v>1638982</v>
+        <v>1616748</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="0"/>
-        <v>676664</v>
+        <f t="shared" ref="G4:G7" si="4">D4-F4-E4</f>
+        <v>668690</v>
       </c>
       <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.56920431000945304</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I8" si="5">F4/D4</f>
+        <v>0.56920431000945304</v>
+      </c>
+      <c r="J4" s="4">
+        <v>539078</v>
+      </c>
+      <c r="K4" s="4">
+        <v>527998</v>
+      </c>
+      <c r="L4" s="4">
+        <v>529590</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33762728084646382</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33068782074648045</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33168489840705573</v>
+      </c>
+      <c r="P4">
+        <v>41.384</v>
+      </c>
+      <c r="Q4" s="27">
         <f t="shared" si="2"/>
-        <v>0.70778607783745873</v>
-      </c>
-      <c r="I4" s="4">
-        <v>546050</v>
-      </c>
-      <c r="J4" s="4">
-        <v>535222</v>
-      </c>
-      <c r="K4" s="4">
-        <v>537347</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33735548637449581</v>
-      </c>
-      <c r="M4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33066583303421004</v>
-      </c>
-      <c r="N4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33197868059129421</v>
-      </c>
-      <c r="O4" s="21">
-        <v>41.414000000000001</v>
-      </c>
-      <c r="P4" s="29">
-        <f t="shared" si="3"/>
-        <v>14.409560817017297</v>
-      </c>
-      <c r="Q4" s="29">
-        <f t="shared" ref="Q4:Q6" si="4">P4/60</f>
-        <v>0.24015934695028829</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <v>14.56995843844013</v>
+      </c>
+      <c r="R4" s="27">
+        <f t="shared" ref="R4:R6" si="6">Q4/60</f>
+        <v>0.24283264064066884</v>
+      </c>
+      <c r="S4" s="3">
+        <f>(J4+K4+L4)/D4</f>
+        <v>0.56213409192128472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -1120,56 +1184,64 @@
         <v>21</v>
       </c>
       <c r="D5" s="4">
-        <v>1393116</v>
+        <v>1374577</v>
       </c>
       <c r="E5" s="4">
-        <v>300316</v>
+        <v>298225</v>
       </c>
       <c r="F5" s="4">
-        <v>828189</v>
+        <v>816217</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="0"/>
-        <v>264611</v>
+        <f t="shared" si="4"/>
+        <v>260135</v>
       </c>
       <c r="H5" s="3">
-        <f>F5/(F5+G5)</f>
-        <v>0.7578596266471449</v>
-      </c>
-      <c r="I5" s="4">
-        <v>271713</v>
+        <f>F5/D5</f>
+        <v>0.59379503658216315</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.59379503658216315</v>
       </c>
       <c r="J5" s="4">
-        <v>272581</v>
+        <v>267992</v>
       </c>
       <c r="K5" s="4">
-        <v>272730</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33256428207739308</v>
+        <v>268730</v>
+      </c>
+      <c r="L5" s="4">
+        <v>268478</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33362667436941879</v>
+        <f t="shared" si="0"/>
+        <v>0.3328266269249876</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33380904355318813</v>
-      </c>
-      <c r="O5" s="21">
-        <v>31.548999999999999</v>
-      </c>
-      <c r="P5" s="29">
-        <f>O5/D5*1000000</f>
-        <v>22.646355364520971</v>
-      </c>
-      <c r="Q5" s="29">
-        <f t="shared" si="4"/>
-        <v>0.37743925607534951</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.33374316939890708</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33343020367610532</v>
+      </c>
+      <c r="P5">
+        <v>29.991</v>
+      </c>
+      <c r="Q5" s="27">
+        <f>P5/D5*1000000</f>
+        <v>21.818348481023616</v>
+      </c>
+      <c r="R5" s="27">
+        <f t="shared" si="6"/>
+        <v>0.3636391413503936</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.58578020729286173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1180,56 +1252,64 @@
         <v>21</v>
       </c>
       <c r="D6" s="4">
-        <v>3385387</v>
+        <v>3340992</v>
       </c>
       <c r="E6" s="4">
-        <v>585399</v>
+        <v>581460</v>
       </c>
       <c r="F6" s="4">
-        <v>2087743</v>
+        <v>2057780</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="0"/>
-        <v>712245</v>
+        <f t="shared" si="4"/>
+        <v>701752</v>
       </c>
       <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.61591886481619829</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.61591886481619829</v>
+      </c>
+      <c r="J6" s="4">
+        <v>674853</v>
+      </c>
+      <c r="K6" s="4">
+        <v>688030</v>
+      </c>
+      <c r="L6" s="4">
+        <v>671700</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33169106396740755</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33816757537048131</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33014136066211108</v>
+      </c>
+      <c r="P6">
+        <v>44.423999999999999</v>
+      </c>
+      <c r="Q6" s="27">
         <f t="shared" si="2"/>
-        <v>0.74562569553869518</v>
-      </c>
-      <c r="I6" s="4">
-        <v>684353</v>
-      </c>
-      <c r="J6" s="4">
-        <v>697846</v>
-      </c>
-      <c r="K6" s="4">
-        <v>681986</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33153665974706725</v>
-      </c>
-      <c r="M6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33807338005072218</v>
-      </c>
-      <c r="N6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33038996020221056</v>
-      </c>
-      <c r="O6" s="21">
-        <v>43.750999999999998</v>
-      </c>
-      <c r="P6" s="29">
-        <f t="shared" si="3"/>
-        <v>12.923485557190359</v>
-      </c>
-      <c r="Q6" s="29">
-        <f t="shared" si="4"/>
-        <v>0.21539142595317265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.296649617838057</v>
+      </c>
+      <c r="R6" s="27">
+        <f t="shared" si="6"/>
+        <v>0.22161082696396761</v>
+      </c>
+      <c r="S6" s="3">
+        <f>(J6+K6+L6)/D6</f>
+        <v>0.60897571739172074</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
@@ -1240,56 +1320,64 @@
         <v>21</v>
       </c>
       <c r="D7" s="12">
-        <v>3217619</v>
-      </c>
-      <c r="E7" s="7">
-        <v>505678</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1955063</v>
+        <v>3176144</v>
+      </c>
+      <c r="E7" s="4">
+        <v>502540</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1927315</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="0"/>
-        <v>756878</v>
+        <f t="shared" si="4"/>
+        <v>746289</v>
       </c>
       <c r="H7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.60680970384214317</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.60680970384214317</v>
+      </c>
+      <c r="J7" s="12">
+        <v>626793</v>
+      </c>
+      <c r="K7" s="12">
+        <v>639436</v>
+      </c>
+      <c r="L7" s="12">
+        <v>639157</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3289585417338009</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33559394264469244</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3354475156215066</v>
+      </c>
+      <c r="P7">
+        <v>41.088000000000001</v>
+      </c>
+      <c r="Q7" s="27">
         <f t="shared" si="2"/>
-        <v>0.72090912007303998</v>
-      </c>
-      <c r="I7" s="12">
-        <v>635469</v>
-      </c>
-      <c r="J7" s="12">
-        <v>648377</v>
-      </c>
-      <c r="K7" s="12">
-        <v>648970</v>
-      </c>
-      <c r="L7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.32877883875133485</v>
-      </c>
-      <c r="M7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.3354571775068087</v>
-      </c>
-      <c r="N7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.33576398374185645</v>
-      </c>
-      <c r="O7" s="22">
-        <v>43.506999999999998</v>
-      </c>
-      <c r="P7" s="29">
-        <f t="shared" si="3"/>
-        <v>13.521489026513082</v>
-      </c>
-      <c r="Q7" s="29">
-        <f>P7/60</f>
-        <v>0.2253581504418847</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+        <v>12.936441168914255</v>
+      </c>
+      <c r="R7" s="27">
+        <f>Q7/60</f>
+        <v>0.2156073528152376</v>
+      </c>
+      <c r="S7" s="3">
+        <f>(J7+K7+L7)/D7</f>
+        <v>0.5999054199053947</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
@@ -1300,47 +1388,55 @@
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="17">
-        <f t="shared" ref="H8:N8" si="5">AVERAGE(H2:H7)</f>
-        <v>0.73404857980543836</v>
-      </c>
-      <c r="I8" s="18">
-        <f t="shared" si="5"/>
-        <v>464208.83333333331</v>
+        <f t="shared" ref="H8:O8" si="7">AVERAGE(H2:H7)</f>
+        <v>0.59579516020884027</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.59579516020884027</v>
       </c>
       <c r="J8" s="18">
-        <f t="shared" si="5"/>
-        <v>467005.5</v>
+        <f t="shared" si="7"/>
+        <v>457887.33333333331</v>
       </c>
       <c r="K8" s="18">
-        <f t="shared" si="5"/>
-        <v>464992.33333333331</v>
-      </c>
-      <c r="L8" s="17">
-        <f t="shared" si="5"/>
-        <v>0.33266470166524548</v>
+        <f t="shared" si="7"/>
+        <v>460510.16666666669</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="7"/>
+        <v>458016.16666666669</v>
       </c>
       <c r="M8" s="17">
-        <f t="shared" si="5"/>
-        <v>0.33407129522063972</v>
+        <f t="shared" si="7"/>
+        <v>0.33285588898628243</v>
       </c>
       <c r="N8" s="17">
-        <f t="shared" si="5"/>
-        <v>0.3332640031141148</v>
-      </c>
-      <c r="O8" s="23">
-        <f t="shared" ref="O8:P8" si="6">AVERAGE(O2:O7)</f>
-        <v>37.098333333333336</v>
-      </c>
-      <c r="P8" s="23">
-        <f t="shared" si="6"/>
-        <v>17.077357220973564</v>
-      </c>
-      <c r="Q8" s="23">
-        <f t="shared" ref="Q8" si="7">AVERAGE(Q2:Q7)</f>
-        <v>0.28462262034955943</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>0.3341636323316039</v>
+      </c>
+      <c r="O8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.33298047868211361</v>
+      </c>
+      <c r="P8" s="21">
+        <f t="shared" ref="P8:Q8" si="8">AVERAGE(P2:P7)</f>
+        <v>36.594999999999999</v>
+      </c>
+      <c r="Q8" s="21">
+        <f t="shared" si="8"/>
+        <v>17.068457561117523</v>
+      </c>
+      <c r="R8" s="21">
+        <f t="shared" ref="R8:S8" si="9">AVERAGE(R2:R7)</f>
+        <v>0.28447429268529206</v>
+      </c>
+      <c r="S8" s="17">
+        <f t="shared" si="9"/>
+        <v>0.58842730944217791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -1351,45 +1447,84 @@
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="13">
-        <f t="shared" ref="H9:N9" si="8">STDEV(H2:H7)</f>
-        <v>1.7743982528045446E-2</v>
-      </c>
-      <c r="I9" s="19">
-        <f t="shared" si="8"/>
-        <v>186093.50710480646</v>
+        <f t="shared" ref="H9:O9" si="10">STDEV(H2:H7)</f>
+        <v>1.648697366076857E-2</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="10"/>
+        <v>1.648697366076857E-2</v>
       </c>
       <c r="J9" s="19">
-        <f t="shared" si="8"/>
-        <v>190497.79561637976</v>
+        <f t="shared" si="10"/>
+        <v>183578.47734270664</v>
       </c>
       <c r="K9" s="19">
-        <f t="shared" si="8"/>
-        <v>186825.55247360209</v>
-      </c>
-      <c r="L9" s="13">
-        <f t="shared" si="8"/>
-        <v>2.8164117333731539E-3</v>
+        <f t="shared" si="10"/>
+        <v>187875.4740932585</v>
+      </c>
+      <c r="L9" s="19">
+        <f t="shared" si="10"/>
+        <v>184055.93685444284</v>
       </c>
       <c r="M9" s="13">
-        <f t="shared" si="8"/>
-        <v>2.4929785873709243E-3</v>
+        <f t="shared" si="10"/>
+        <v>2.8435522167663384E-3</v>
       </c>
       <c r="N9" s="13">
-        <f t="shared" si="8"/>
-        <v>1.8737337932607115E-3</v>
-      </c>
-      <c r="O9" s="24">
-        <f t="shared" ref="O9:P9" si="9">STDEV(O2:O7)</f>
-        <v>6.7862259221651682</v>
-      </c>
-      <c r="P9" s="24">
-        <f t="shared" si="9"/>
-        <v>4.355036229532586</v>
-      </c>
-      <c r="Q9" s="24">
-        <f t="shared" ref="Q9" si="10">STDEV(Q2:Q7)</f>
-        <v>7.2583937158876427E-2</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>2.5173970746338024E-3</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="10"/>
+        <v>1.8523259959090524E-3</v>
+      </c>
+      <c r="P9" s="22">
+        <f t="shared" ref="P9:Q9" si="11">STDEV(P2:P7)</f>
+        <v>6.693207960313214</v>
+      </c>
+      <c r="Q9" s="22">
+        <f t="shared" si="11"/>
+        <v>4.3519079776455873</v>
+      </c>
+      <c r="R9" s="22">
+        <f t="shared" ref="R9:S9" si="12">STDEV(R2:R7)</f>
+        <v>7.2531799627426466E-2</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" si="12"/>
+        <v>1.6704081634077758E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="41"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1397,16 +1532,634 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004FEFD4-A36D-7843-8AFA-92A18F957172}">
-  <dimension ref="A1:S21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A77191-EB84-9140-9493-17DED251511A}">
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="L1" zoomScale="193" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="7" width="17.33203125" customWidth="1"/>
+    <col min="10" max="12" width="20.33203125" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2052039</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2-F2-G2</f>
+        <v>184762</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1252773</v>
+      </c>
+      <c r="G2" s="4">
+        <v>614504</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2/(F2+G2)</f>
+        <v>0.67090902956551168</v>
+      </c>
+      <c r="I2" s="3">
+        <f>F2/D2</f>
+        <v>0.61050155479501123</v>
+      </c>
+      <c r="J2" s="4">
+        <v>410809</v>
+      </c>
+      <c r="K2" s="4">
+        <v>411883</v>
+      </c>
+      <c r="L2" s="4">
+        <v>411971</v>
+      </c>
+      <c r="M2" s="3">
+        <f t="shared" ref="M2:O7" si="0">J2/($J2+$K2+$L2)</f>
+        <v>0.33272965983430297</v>
+      </c>
+      <c r="N2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33359953282798627</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33367080733771076</v>
+      </c>
+      <c r="P2">
+        <v>196.32499999999999</v>
+      </c>
+      <c r="Q2" s="27">
+        <f>P2/D2*1000000</f>
+        <v>95.673132918039073</v>
+      </c>
+      <c r="R2" s="27">
+        <f>Q2/60</f>
+        <v>1.5945522153006513</v>
+      </c>
+      <c r="S2" s="3">
+        <f>(J2+K2+L2)/D2</f>
+        <v>0.60167618646624166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1225463</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E7" si="1">D3-F3-G3</f>
+        <v>86285</v>
+      </c>
+      <c r="F3" s="4">
+        <v>772166</v>
+      </c>
+      <c r="G3" s="4">
+        <v>367012</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H7" si="2">F3/(F3+G3)</f>
+        <v>0.67782734568258862</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I7" si="3">F3/D3</f>
+        <v>0.63010143921113893</v>
+      </c>
+      <c r="J3" s="4">
+        <v>252754</v>
+      </c>
+      <c r="K3" s="4">
+        <v>255312</v>
+      </c>
+      <c r="L3" s="4">
+        <v>254949</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33125692155462211</v>
+      </c>
+      <c r="N3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33460941134840078</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33413366709697712</v>
+      </c>
+      <c r="P3">
+        <v>199.75399999999999</v>
+      </c>
+      <c r="Q3" s="27">
+        <f t="shared" ref="Q3:Q7" si="4">P3/D3*1000000</f>
+        <v>163.00288135994313</v>
+      </c>
+      <c r="R3" s="27">
+        <f>Q3/60</f>
+        <v>2.7167146893323855</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S7" si="5">(J3+K3+L3)/D3</f>
+        <v>0.62263405749500389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2840365</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="1"/>
+        <v>206494</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1701256</v>
+      </c>
+      <c r="G4" s="4">
+        <v>932615</v>
+      </c>
+      <c r="H4" s="3">
+        <f>F4/(F4+G4)</f>
+        <v>0.645914701213537</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.59895682421097285</v>
+      </c>
+      <c r="J4" s="4">
+        <v>565304</v>
+      </c>
+      <c r="K4" s="4">
+        <v>557482</v>
+      </c>
+      <c r="L4" s="4">
+        <v>557528</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33642759627069702</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33177251394679802</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33179988978250496</v>
+      </c>
+      <c r="P4">
+        <v>204.89400000000001</v>
+      </c>
+      <c r="Q4" s="27">
+        <f t="shared" si="4"/>
+        <v>72.136503583166245</v>
+      </c>
+      <c r="R4" s="27">
+        <f t="shared" ref="R4:R6" si="6">Q4/60</f>
+        <v>1.2022750597194374</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5915838281347644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1374577</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="1"/>
+        <v>131876</v>
+      </c>
+      <c r="F5" s="4">
+        <v>858110</v>
+      </c>
+      <c r="G5" s="4">
+        <v>384591</v>
+      </c>
+      <c r="H5" s="3">
+        <f>F5/(F5+G5)</f>
+        <v>0.69052008487962913</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.62427204878300746</v>
+      </c>
+      <c r="J5" s="4">
+        <v>280754</v>
+      </c>
+      <c r="K5" s="4">
+        <v>282722</v>
+      </c>
+      <c r="L5" s="4">
+        <v>282395</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3319111306570387</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33423772655641343</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33385114278654782</v>
+      </c>
+      <c r="P5">
+        <v>80.781999999999996</v>
+      </c>
+      <c r="Q5" s="27">
+        <f>P5/D5*1000000</f>
+        <v>58.768624820581159</v>
+      </c>
+      <c r="R5" s="27">
+        <f t="shared" si="6"/>
+        <v>0.97947708034301928</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.61536821873201719</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3340992</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="1"/>
+        <v>244900</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2142498</v>
+      </c>
+      <c r="G6" s="4">
+        <v>953594</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.69200075449954335</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.64127600425262921</v>
+      </c>
+      <c r="J6" s="4">
+        <v>700864</v>
+      </c>
+      <c r="K6" s="4">
+        <v>717466</v>
+      </c>
+      <c r="L6" s="4">
+        <v>699399</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3309507496001613</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33879027958723706</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33025897081260164</v>
+      </c>
+      <c r="P6">
+        <v>84.796999999999997</v>
+      </c>
+      <c r="Q6" s="27">
+        <f t="shared" si="4"/>
+        <v>25.380785108135548</v>
+      </c>
+      <c r="R6" s="27">
+        <f t="shared" si="6"/>
+        <v>0.42301308513559249</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.63386233789245827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3176144</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="1"/>
+        <v>203532</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1998311</v>
+      </c>
+      <c r="G7" s="4">
+        <v>974301</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.6722407767983174</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.62916259464306401</v>
+      </c>
+      <c r="J7" s="12">
+        <v>648052</v>
+      </c>
+      <c r="K7" s="12">
+        <v>664511</v>
+      </c>
+      <c r="L7" s="12">
+        <v>663023</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.32803026545035247</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33636146439588049</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33560827015376704</v>
+      </c>
+      <c r="P7">
+        <v>218.333</v>
+      </c>
+      <c r="Q7" s="27">
+        <f t="shared" si="4"/>
+        <v>68.741530610702796</v>
+      </c>
+      <c r="R7" s="27">
+        <f>Q7/60</f>
+        <v>1.1456921768450465</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.62200769234644271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17">
+        <f t="shared" ref="H8:S8" si="7">AVERAGE(H2:H7)</f>
+        <v>0.67490211543985446</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.62237841098263735</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="7"/>
+        <v>476422.83333333331</v>
+      </c>
+      <c r="K8" s="18">
+        <f t="shared" si="7"/>
+        <v>481562.66666666669</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="7"/>
+        <v>478210.83333333331</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.3318843872278624</v>
+      </c>
+      <c r="N8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.33489515477711929</v>
+      </c>
+      <c r="O8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.3332204579950182</v>
+      </c>
+      <c r="P8" s="21">
+        <f t="shared" si="7"/>
+        <v>164.14750000000001</v>
+      </c>
+      <c r="Q8" s="21">
+        <f t="shared" si="7"/>
+        <v>80.617243066761333</v>
+      </c>
+      <c r="R8" s="21">
+        <f t="shared" si="7"/>
+        <v>1.3436207177793555</v>
+      </c>
+      <c r="S8" s="17">
+        <f t="shared" si="7"/>
+        <v>0.61452205351115463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="13">
+        <f t="shared" ref="H9:S9" si="8">STDEV(H2:H7)</f>
+        <v>1.6781770113913411E-2</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="8"/>
+        <v>1.5205299393815479E-2</v>
+      </c>
+      <c r="J9" s="19">
+        <f t="shared" si="8"/>
+        <v>189920.76474194878</v>
+      </c>
+      <c r="K9" s="19">
+        <f t="shared" si="8"/>
+        <v>195175.02471132582</v>
+      </c>
+      <c r="L9" s="19">
+        <f t="shared" si="8"/>
+        <v>190760.77022115068</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" si="8"/>
+        <v>2.7377215513608301E-3</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" si="8"/>
+        <v>2.4193157853892372E-3</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="8"/>
+        <v>1.8933882847488219E-3</v>
+      </c>
+      <c r="P9" s="22">
+        <f t="shared" si="8"/>
+        <v>63.475772482893042</v>
+      </c>
+      <c r="Q9" s="22">
+        <f t="shared" si="8"/>
+        <v>46.379860094223503</v>
+      </c>
+      <c r="R9" s="22">
+        <f t="shared" si="8"/>
+        <v>0.77299766823705851</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" si="8"/>
+        <v>1.5412854871766673E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004FEFD4-A36D-7843-8AFA-92A18F957172}">
+  <dimension ref="A1:S21"/>
+  <sheetViews>
+    <sheetView topLeftCell="H10" zoomScale="185" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="12" width="16.1640625" customWidth="1"/>
@@ -1414,61 +2167,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="24" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1485,29 +2238,56 @@
       <c r="D2" s="4">
         <v>2078810</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="3" t="e">
+      <c r="E2" s="42">
+        <v>1191185</v>
+      </c>
+      <c r="F2" s="7">
+        <v>498130</v>
+      </c>
+      <c r="G2" s="30">
+        <f>D2-E2-F2</f>
+        <v>389495</v>
+      </c>
+      <c r="H2">
+        <v>1227784</v>
+      </c>
+      <c r="I2" s="4">
+        <v>477607</v>
+      </c>
+      <c r="J2" s="4">
+        <f>D2-H2-I2</f>
+        <v>373419</v>
+      </c>
+      <c r="K2" s="42">
+        <v>1228922</v>
+      </c>
+      <c r="L2" s="7">
+        <v>497422</v>
+      </c>
+      <c r="M2" s="30">
+        <f>D2-K2-L2</f>
+        <v>352466</v>
+      </c>
+      <c r="N2" s="4">
+        <v>182954</v>
+      </c>
+      <c r="O2" s="4">
+        <v>187373</v>
+      </c>
+      <c r="P2" s="4">
+        <v>207778</v>
+      </c>
+      <c r="Q2" s="3">
         <f>N2/(N2+O2+P2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R2" s="3" t="e">
+        <v>0.31647192119078715</v>
+      </c>
+      <c r="R2" s="3">
         <f>O2/(N2+O2+P2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S2" s="3" t="e">
+        <v>0.32411586130547221</v>
+      </c>
+      <c r="S2" s="3">
         <f>P2/(N2+O2+P2)</f>
-        <v>#DIV/0!</v>
+        <v>0.35941221750374069</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -1523,29 +2303,56 @@
       <c r="D3" s="4">
         <v>1241292</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="3" t="e">
-        <f t="shared" ref="Q3:Q7" si="0">N3/(N3+O3+P3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R3" s="3" t="e">
-        <f t="shared" ref="R3:R7" si="1">O3/(N3+O3+P3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S3" s="3" t="e">
-        <f t="shared" ref="S3:S7" si="2">P3/(N3+O3+P3)</f>
-        <v>#DIV/0!</v>
+      <c r="E3" s="32">
+        <v>740747</v>
+      </c>
+      <c r="F3" s="7">
+        <v>267473</v>
+      </c>
+      <c r="G3" s="30">
+        <f t="shared" ref="G3:G7" si="0">D3-E3-F3</f>
+        <v>233072</v>
+      </c>
+      <c r="H3">
+        <v>782782</v>
+      </c>
+      <c r="I3" s="4">
+        <v>232553</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J7" si="1">D3-H3-I3</f>
+        <v>225957</v>
+      </c>
+      <c r="K3" s="32">
+        <v>762487</v>
+      </c>
+      <c r="L3" s="7">
+        <v>264296</v>
+      </c>
+      <c r="M3" s="30">
+        <f t="shared" ref="M3:M7" si="2">D3-K3-L3</f>
+        <v>214509</v>
+      </c>
+      <c r="N3" s="4">
+        <v>116346</v>
+      </c>
+      <c r="O3" s="4">
+        <v>120896</v>
+      </c>
+      <c r="P3" s="4">
+        <v>128959</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q7" si="3">N3/(N3+O3+P3)</f>
+        <v>0.31771076539932985</v>
+      </c>
+      <c r="R3" s="3">
+        <f t="shared" ref="R3:R7" si="4">O3/(N3+O3+P3)</f>
+        <v>0.33013563589394895</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S7" si="5">P3/(N3+O3+P3)</f>
+        <v>0.35215359870672119</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1561,29 +2368,56 @@
       <c r="D4" s="4">
         <v>2874064</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="3" t="e">
+      <c r="E4" s="32">
+        <v>1674711</v>
+      </c>
+      <c r="F4" s="7">
+        <v>688541</v>
+      </c>
+      <c r="G4" s="30">
+        <f t="shared" si="0"/>
+        <v>510812</v>
+      </c>
+      <c r="H4">
+        <v>1803367</v>
+      </c>
+      <c r="I4" s="4">
+        <v>573611</v>
+      </c>
+      <c r="J4" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S4" s="3" t="e">
+        <v>497086</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1732844</v>
+      </c>
+      <c r="L4" s="7">
+        <v>674657</v>
+      </c>
+      <c r="M4" s="30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>466563</v>
+      </c>
+      <c r="N4" s="4">
+        <v>269473</v>
+      </c>
+      <c r="O4" s="4">
+        <v>281733</v>
+      </c>
+      <c r="P4" s="4">
+        <v>300975</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.31621568657362698</v>
+      </c>
+      <c r="R4" s="3">
+        <f t="shared" si="4"/>
+        <v>0.33060230162371607</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.35318201180265696</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1599,29 +2433,56 @@
       <c r="D5" s="4">
         <v>1393116</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" s="3" t="e">
+      <c r="E5" s="32">
+        <v>794443</v>
+      </c>
+      <c r="F5" s="7">
+        <v>316903</v>
+      </c>
+      <c r="G5" s="30">
+        <f t="shared" si="0"/>
+        <v>281770</v>
+      </c>
+      <c r="H5">
+        <v>822067</v>
+      </c>
+      <c r="I5" s="4">
+        <v>306821</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S5" s="3" t="e">
+        <v>264228</v>
+      </c>
+      <c r="K5" s="32">
+        <v>819859</v>
+      </c>
+      <c r="L5" s="7">
+        <v>319842</v>
+      </c>
+      <c r="M5" s="30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>253415</v>
+      </c>
+      <c r="N5" s="4">
+        <v>120733</v>
+      </c>
+      <c r="O5" s="4">
+        <v>121168</v>
+      </c>
+      <c r="P5" s="4">
+        <v>139820</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.31628597850262363</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" si="4"/>
+        <v>0.31742555426607394</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.36628846723130243</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -1637,29 +2498,56 @@
       <c r="D6" s="4">
         <v>3385387</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R6" s="3" t="e">
+      <c r="E6" s="32">
+        <v>2037031</v>
+      </c>
+      <c r="F6" s="7">
+        <v>697859</v>
+      </c>
+      <c r="G6" s="30">
+        <f t="shared" si="0"/>
+        <v>650497</v>
+      </c>
+      <c r="H6">
+        <v>2135715</v>
+      </c>
+      <c r="I6" s="4">
+        <v>627022</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" s="3" t="e">
+        <v>622650</v>
+      </c>
+      <c r="K6" s="32">
+        <v>2094869</v>
+      </c>
+      <c r="L6" s="7">
+        <v>696599</v>
+      </c>
+      <c r="M6" s="30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>593919</v>
+      </c>
+      <c r="N6" s="4">
+        <v>318520</v>
+      </c>
+      <c r="O6" s="4">
+        <v>334239</v>
+      </c>
+      <c r="P6" s="4">
+        <v>358535</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.31496281002359355</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" si="4"/>
+        <v>0.3305062622738788</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.35453092770252764</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1675,29 +2563,56 @@
       <c r="D7" s="12">
         <v>3217619</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="3" t="e">
+      <c r="E7" s="35">
+        <v>1919549</v>
+      </c>
+      <c r="F7" s="12">
+        <v>698892</v>
+      </c>
+      <c r="G7" s="31">
+        <f t="shared" si="0"/>
+        <v>599178</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2035418</v>
+      </c>
+      <c r="I7" s="12">
+        <v>597150</v>
+      </c>
+      <c r="J7" s="12">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="3" t="e">
+        <v>585051</v>
+      </c>
+      <c r="K7" s="35">
+        <v>1971697</v>
+      </c>
+      <c r="L7" s="12">
+        <v>698399</v>
+      </c>
+      <c r="M7" s="31">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>547523</v>
+      </c>
+      <c r="N7" s="4">
+        <v>297053</v>
+      </c>
+      <c r="O7" s="4">
+        <v>313147</v>
+      </c>
+      <c r="P7" s="4">
+        <v>334059</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.31458847625492581</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" si="4"/>
+        <v>0.33163252878712302</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.35377899495795118</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1707,24 +2622,24 @@
         <v>11</v>
       </c>
       <c r="D8" s="18"/>
-      <c r="E8" s="36"/>
-      <c r="G8" s="37"/>
-      <c r="K8" s="36"/>
-      <c r="M8" s="37"/>
+      <c r="E8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="K8" s="32"/>
+      <c r="M8" s="33"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="38" t="e">
+      <c r="Q8" s="34">
         <f>AVERAGE(Q2:Q7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="38" t="e">
-        <f t="shared" ref="R8:S8" si="3">AVERAGE(R2:R7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S8" s="38" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.31603927299081452</v>
+      </c>
+      <c r="R8" s="34">
+        <f t="shared" ref="R8:S8" si="6">AVERAGE(R2:R7)</f>
+        <v>0.32740302402503546</v>
+      </c>
+      <c r="S8" s="34">
+        <f t="shared" si="6"/>
+        <v>0.35655770298415002</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1734,68 +2649,64 @@
         <v>12</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="39"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="40"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="39"/>
+      <c r="K9" s="35"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="40"/>
+      <c r="M9" s="36"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="13" t="e">
+      <c r="Q9" s="13">
         <f>STDEV(Q2:Q7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="13" t="e">
-        <f t="shared" ref="R9:S9" si="4">STDEV(R2:R7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="13" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.1257566688308073E-3</v>
+      </c>
+      <c r="R9" s="13">
+        <f t="shared" ref="R9:S9" si="7">STDEV(R2:R7)</f>
+        <v>5.5781123057362372E-3</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" si="7"/>
+        <v>5.3936349107544862E-3</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="37" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
@@ -1810,15 +2721,23 @@
       <c r="D14" s="4">
         <v>2078810</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="29">
+      <c r="E14" s="32">
+        <v>167.36500000000001</v>
+      </c>
+      <c r="F14">
+        <v>4733.1850000000004</v>
+      </c>
+      <c r="G14" s="38">
+        <v>101.28400000000001</v>
+      </c>
+      <c r="H14" s="43">
+        <f>E14+F14+G14</f>
+        <v>5001.8339999999998</v>
+      </c>
+      <c r="I14" s="27">
         <f>(H14/60)/D14*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="29"/>
+        <v>40.101740899841737</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -1833,15 +2752,23 @@
       <c r="D15" s="4">
         <v>1241292</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="29">
-        <f t="shared" ref="I15:I19" si="5">(H15/60)/D15*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="29"/>
+      <c r="E15" s="32">
+        <v>137.36199999999999</v>
+      </c>
+      <c r="F15">
+        <v>3256.317</v>
+      </c>
+      <c r="G15" s="38">
+        <v>38.593000000000004</v>
+      </c>
+      <c r="H15" s="43">
+        <f t="shared" ref="H15:H19" si="8">E15+F15+G15</f>
+        <v>3432.2719999999999</v>
+      </c>
+      <c r="I15" s="27">
+        <f t="shared" ref="I15:I19" si="9">(H15/60)/D15*1000000</f>
+        <v>46.08467091815087</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -1856,15 +2783,23 @@
       <c r="D16" s="4">
         <v>2874064</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="29">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="29"/>
+      <c r="E16" s="32">
+        <v>187.96</v>
+      </c>
+      <c r="F16">
+        <v>4354.223</v>
+      </c>
+      <c r="G16" s="38">
+        <v>91.346000000000004</v>
+      </c>
+      <c r="H16" s="43">
+        <f t="shared" si="8"/>
+        <v>4633.5290000000005</v>
+      </c>
+      <c r="I16" s="27">
+        <f>(H16/60)/D16*1000000</f>
+        <v>26.869785548732853</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -1879,15 +2814,23 @@
       <c r="D17" s="4">
         <v>1393116</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="29">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="29"/>
+      <c r="E17" s="32">
+        <v>128.63900000000001</v>
+      </c>
+      <c r="F17">
+        <v>4285.3530000000001</v>
+      </c>
+      <c r="G17" s="38">
+        <v>61.585999999999999</v>
+      </c>
+      <c r="H17" s="43">
+        <f t="shared" si="8"/>
+        <v>4475.5780000000004</v>
+      </c>
+      <c r="I17" s="27">
+        <f t="shared" si="9"/>
+        <v>53.543973844724107</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
@@ -1902,15 +2845,23 @@
       <c r="D18" s="4">
         <v>3385387</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="29">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="29"/>
+      <c r="E18" s="32">
+        <v>161.41399999999999</v>
+      </c>
+      <c r="F18">
+        <v>3650.2660000000001</v>
+      </c>
+      <c r="G18" s="38">
+        <v>39.314999999999998</v>
+      </c>
+      <c r="H18" s="43">
+        <f t="shared" si="8"/>
+        <v>3850.9950000000003</v>
+      </c>
+      <c r="I18" s="27">
+        <f t="shared" si="9"/>
+        <v>18.958910753777928</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
@@ -1925,15 +2876,24 @@
       <c r="D19" s="12">
         <v>3217619</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="44">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="29"/>
+      <c r="E19" s="35">
+        <v>186.86099999999999</v>
+      </c>
+      <c r="F19" s="9">
+        <v>4934.5069999999996</v>
+      </c>
+      <c r="G19" s="39">
+        <v>106.43600000000001</v>
+      </c>
+      <c r="H19" s="44">
+        <f t="shared" si="8"/>
+        <v>5227.8039999999992</v>
+      </c>
+      <c r="I19" s="40">
+        <f t="shared" si="9"/>
+        <v>27.079050274960039</v>
+      </c>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
@@ -1942,11 +2902,13 @@
         <v>11</v>
       </c>
       <c r="D20" s="18"/>
-      <c r="I20" s="29">
+      <c r="E20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="27">
         <f>AVERAGE(I14:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="29"/>
+        <v>35.439688706697922</v>
+      </c>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
@@ -1955,15 +2917,15 @@
         <v>12</v>
       </c>
       <c r="D21" s="19"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="35"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="44">
+      <c r="H21" s="35"/>
+      <c r="I21" s="40">
         <f>STDEV(I14:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="29"/>
+        <v>13.249717539248222</v>
+      </c>
+      <c r="J21" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>